<commit_message>
support dimension weight from data
</commit_message>
<xml_diff>
--- a/cases/goodhostpital2021/维度导向库.xlsx
+++ b/cases/goodhostpital2021/维度导向库.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="一级指标设置" sheetId="1" state="visible" r:id="rId2"/>
@@ -894,10 +894,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -907,217 +907,147 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>0.3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="n">
         <v>0.3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>0.4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>0.5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="n">
         <v>0.5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="0" t="n">
         <v>0.5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="n">
         <v>0.5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1136,7 +1066,7 @@
   </sheetPr>
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>